<commit_message>
feat(parser): added formula parser for calculation
</commit_message>
<xml_diff>
--- a/ExcelLogic.xlsx
+++ b/ExcelLogic.xlsx
@@ -1,25 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adriankroeger/Documents/apps/ExcelCliProject/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AE45C7-1293-7144-A8F8-74D0D5A40957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10313"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF3553D-0AEE-D74F-BDB1-85F0CDF7CA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="16940" xr2:uid="{B4891A5C-939B-D54F-9D92-B74829655341}"/>
+    <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -47,7 +39,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,9 +81,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -398,26 +398,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5B8549-4CB5-9741-B059-DB3B3AE6C9E1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="261" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="261" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <f>B3*12</f>
         <v>0</v>
       </c>

</xml_diff>